<commit_message>
FEAT: Actualizacion de ventana de Configuracion de Autos, Articulos de Servicio y configuracion de Agntes
</commit_message>
<xml_diff>
--- a/04 Documentacion/Agencias Nissan.xlsx
+++ b/04 Documentacion/Agencias Nissan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -500,6 +500,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -523,24 +541,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,35 +837,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="1" t="s">
         <v>40</v>
       </c>
@@ -877,264 +877,264 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="13">
         <v>234</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="12">
         <v>6000</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="13">
         <v>171</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="11">
         <v>6000</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="9">
         <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="13">
         <v>208</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="9">
         <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="13">
         <v>221</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="9">
         <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="13">
         <v>252</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="9">
         <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="13">
         <v>253</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="9">
         <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="13">
         <v>61</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="12">
         <v>6000</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1145,38 +1145,38 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="13">
         <v>78</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="3" t="s">
         <v>27</v>
       </c>
@@ -1185,38 +1185,38 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="13">
         <v>81</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="3" t="s">
         <v>27</v>
       </c>
@@ -1225,40 +1225,40 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="F29" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
       <c r="E30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="17">
+      <c r="B31" s="13">
         <v>428</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="12">
         <v>6000</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="12" t="s">
         <v>56</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1269,38 +1269,38 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
       <c r="E33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="F33" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B34" s="13">
         <v>433</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
       <c r="E34" s="3" t="s">
         <v>27</v>
       </c>
@@ -1309,38 +1309,38 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
       <c r="E35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="9" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
       <c r="E36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F36" s="9" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B37" s="13">
         <v>374</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
       <c r="E37" s="3" t="s">
         <v>27</v>
       </c>
@@ -1349,38 +1349,38 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
       <c r="E38" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="21" t="s">
+      <c r="F38" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
       <c r="E39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="F39" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="17">
+      <c r="B40" s="13">
         <v>209</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
       <c r="E40" s="3" t="s">
         <v>27</v>
       </c>
@@ -1389,40 +1389,40 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="17"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
       <c r="E41" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="F41" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
       <c r="E42" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F42" s="21" t="s">
+      <c r="F42" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B43" s="13">
         <v>262</v>
       </c>
-      <c r="C43" s="19">
+      <c r="C43" s="14">
         <v>4600</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1433,38 +1433,38 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="18"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="12"/>
       <c r="E44" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F44" s="21" t="s">
+      <c r="F44" s="9" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="18"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="12"/>
       <c r="E45" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F45" s="21" t="s">
+      <c r="F45" s="9" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="17">
+      <c r="B46" s="13">
         <v>263</v>
       </c>
-      <c r="C46" s="19"/>
-      <c r="D46" s="18"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="12"/>
       <c r="E46" s="3" t="s">
         <v>27</v>
       </c>
@@ -1473,38 +1473,38 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="17"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="18"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="12"/>
       <c r="E47" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F47" s="22" t="s">
+      <c r="F47" s="10" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="18"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="12"/>
       <c r="E48" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="F48" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="17">
+      <c r="B49" s="13">
         <v>264</v>
       </c>
-      <c r="C49" s="19"/>
-      <c r="D49" s="18"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="12"/>
       <c r="E49" s="3" t="s">
         <v>27</v>
       </c>
@@ -1514,40 +1514,40 @@
       <c r="I49" s="8"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="18"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="12"/>
       <c r="E50" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="F50" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="17"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="18"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="12"/>
       <c r="E51" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="F51" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="17">
+      <c r="B52" s="13">
         <v>202</v>
       </c>
-      <c r="C52" s="18">
+      <c r="C52" s="12">
         <v>4600</v>
       </c>
-      <c r="D52" s="18" t="s">
+      <c r="D52" s="12" t="s">
         <v>73</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -1558,40 +1558,40 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
       <c r="E53" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F53" s="21" t="s">
+      <c r="F53" s="9" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
       <c r="E54" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="F54" s="9" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="17">
+      <c r="B55" s="13">
         <v>394</v>
       </c>
-      <c r="C55" s="18">
+      <c r="C55" s="12">
         <v>4600</v>
       </c>
-      <c r="D55" s="18" t="s">
+      <c r="D55" s="12" t="s">
         <v>77</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -1602,40 +1602,40 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
       <c r="E56" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F56" s="21" t="s">
+      <c r="F56" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="17"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
       <c r="E57" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F57" s="21" t="s">
+      <c r="F57" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="17">
+      <c r="B58" s="13">
         <v>361</v>
       </c>
-      <c r="C58" s="18">
+      <c r="C58" s="12">
         <v>4600</v>
       </c>
-      <c r="D58" s="18"/>
+      <c r="D58" s="12"/>
       <c r="E58" s="3" t="s">
         <v>27</v>
       </c>
@@ -1644,40 +1644,40 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
       <c r="E59" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F59" s="21" t="s">
+      <c r="F59" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="17"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
       <c r="E60" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F60" s="21" t="s">
+      <c r="F60" s="9" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B61" s="17">
+      <c r="B61" s="13">
         <v>364</v>
       </c>
-      <c r="C61" s="18">
+      <c r="C61" s="12">
         <v>4600</v>
       </c>
-      <c r="D61" s="18"/>
+      <c r="D61" s="12"/>
       <c r="E61" s="3" t="s">
         <v>27</v>
       </c>
@@ -1686,40 +1686,40 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="17"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
+      <c r="A62" s="13"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
       <c r="E62" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F62" s="21" t="s">
+      <c r="F62" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="17"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
       <c r="E63" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F63" s="21" t="s">
+      <c r="F63" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B64" s="17">
+      <c r="B64" s="13">
         <v>366</v>
       </c>
-      <c r="C64" s="18">
+      <c r="C64" s="12">
         <v>4600</v>
       </c>
-      <c r="D64" s="18"/>
+      <c r="D64" s="12"/>
       <c r="E64" s="3" t="s">
         <v>27</v>
       </c>
@@ -1728,40 +1728,40 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="17"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
+      <c r="A65" s="13"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
       <c r="E65" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F65" s="21" t="s">
+      <c r="F65" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="17"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
+      <c r="A66" s="13"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
       <c r="E66" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F66" s="21" t="s">
+      <c r="F66" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B67" s="17">
+      <c r="B67" s="13">
         <v>393</v>
       </c>
-      <c r="C67" s="18">
+      <c r="C67" s="12">
         <v>4600</v>
       </c>
-      <c r="D67" s="18" t="s">
+      <c r="D67" s="12" t="s">
         <v>76</v>
       </c>
       <c r="E67" s="3" t="s">
@@ -1772,40 +1772,40 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="17"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
       <c r="E68" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F68" s="21" t="s">
+      <c r="F68" s="9" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="17"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
+      <c r="A69" s="13"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
       <c r="E69" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F69" s="21" t="s">
+      <c r="F69" s="9" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="17" t="s">
+      <c r="A70" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B70" s="17">
+      <c r="B70" s="13">
         <v>215</v>
       </c>
-      <c r="C70" s="18">
+      <c r="C70" s="12">
         <v>4600</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="D70" s="12" t="s">
         <v>46</v>
       </c>
       <c r="E70" s="3" t="s">
@@ -1816,10 +1816,10 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="17"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
+      <c r="A71" s="13"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
       <c r="E71" s="3" t="s">
         <v>28</v>
       </c>
@@ -1828,10 +1828,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
       <c r="E72" s="3" t="s">
         <v>29</v>
       </c>
@@ -1840,38 +1840,38 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="17" t="s">
+      <c r="A73" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B73" s="17">
+      <c r="B73" s="13">
         <v>243</v>
       </c>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
       <c r="E73" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F73" s="21">
+      <c r="F73" s="9">
         <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
       <c r="E74" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F74" s="21" t="s">
+      <c r="F74" s="9" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="17"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
+      <c r="A75" s="13"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
       <c r="E75" s="3" t="s">
         <v>29</v>
       </c>
@@ -1905,6 +1905,64 @@
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="D67:D69"/>
+    <mergeCell ref="D55:D66"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="C67:C69"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="C43:C51"/>
+    <mergeCell ref="C70:C75"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="D22:D30"/>
+    <mergeCell ref="D31:D42"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="D43:D51"/>
+    <mergeCell ref="C31:C42"/>
+    <mergeCell ref="C22:C30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C21"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="D7:D21"/>
     <mergeCell ref="D4:D6"/>
     <mergeCell ref="B73:B75"/>
@@ -1921,64 +1979,6 @@
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C21"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="D22:D30"/>
-    <mergeCell ref="D31:D42"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="D43:D51"/>
-    <mergeCell ref="C31:C42"/>
-    <mergeCell ref="C22:C30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="C43:C51"/>
-    <mergeCell ref="C70:C75"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="C67:C69"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="D67:D69"/>
-    <mergeCell ref="D55:D66"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion a sp de crear clientes
</commit_message>
<xml_diff>
--- a/04 Documentacion/Agencias Nissan.xlsx
+++ b/04 Documentacion/Agencias Nissan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -506,24 +506,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -540,6 +522,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:B42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,35 +837,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="1" t="s">
         <v>40</v>
       </c>
@@ -877,16 +877,16 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="20">
         <v>234</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="17">
         <v>6000</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="17" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -897,10 +897,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
@@ -909,10 +909,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="3" t="s">
         <v>29</v>
       </c>
@@ -921,16 +921,16 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="20">
         <v>171</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="22">
         <v>6000</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="22" t="s">
         <v>43</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -941,10 +941,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
@@ -953,10 +953,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
@@ -965,14 +965,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="20">
         <v>208</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="3" t="s">
         <v>27</v>
       </c>
@@ -981,10 +981,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
@@ -993,10 +993,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1005,14 +1005,14 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="20">
         <v>221</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="3" t="s">
         <v>27</v>
       </c>
@@ -1021,10 +1021,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="3" t="s">
         <v>28</v>
       </c>
@@ -1033,10 +1033,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1045,14 +1045,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="20">
         <v>252</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="3" t="s">
         <v>27</v>
       </c>
@@ -1061,10 +1061,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
       <c r="E17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1073,10 +1073,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="3" t="s">
         <v>29</v>
       </c>
@@ -1085,14 +1085,14 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="20">
         <v>253</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1101,10 +1101,10 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1113,10 +1113,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
       <c r="E21" s="3" t="s">
         <v>29</v>
       </c>
@@ -1125,16 +1125,16 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="20">
         <v>61</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="17">
         <v>6000</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="17" t="s">
         <v>49</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1145,10 +1145,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
       <c r="E23" s="3" t="s">
         <v>28</v>
       </c>
@@ -1157,10 +1157,10 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
       <c r="E24" s="3" t="s">
         <v>29</v>
       </c>
@@ -1169,14 +1169,14 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="20">
         <v>78</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
       <c r="E25" s="3" t="s">
         <v>27</v>
       </c>
@@ -1185,10 +1185,10 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
       <c r="E26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1197,10 +1197,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
       <c r="E27" s="3" t="s">
         <v>29</v>
       </c>
@@ -1209,14 +1209,14 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B28" s="20">
         <v>81</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
       <c r="E28" s="3" t="s">
         <v>27</v>
       </c>
@@ -1225,10 +1225,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
       <c r="E29" s="3" t="s">
         <v>28</v>
       </c>
@@ -1237,10 +1237,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
       <c r="E30" s="3" t="s">
         <v>29</v>
       </c>
@@ -1249,16 +1249,16 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31" s="20">
         <v>428</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="17">
         <v>6000</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="17" t="s">
         <v>56</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1269,10 +1269,10 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
       <c r="E32" s="3" t="s">
         <v>28</v>
       </c>
@@ -1281,10 +1281,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
       <c r="E33" s="3" t="s">
         <v>29</v>
       </c>
@@ -1293,14 +1293,14 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="20">
         <v>433</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
       <c r="E34" s="3" t="s">
         <v>27</v>
       </c>
@@ -1309,10 +1309,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
       <c r="E35" s="3" t="s">
         <v>28</v>
       </c>
@@ -1321,10 +1321,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
       <c r="E36" s="3" t="s">
         <v>29</v>
       </c>
@@ -1333,14 +1333,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="20">
         <v>374</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
       <c r="E37" s="3" t="s">
         <v>27</v>
       </c>
@@ -1349,10 +1349,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
       <c r="E38" s="3" t="s">
         <v>28</v>
       </c>
@@ -1361,10 +1361,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
       <c r="E39" s="3" t="s">
         <v>29</v>
       </c>
@@ -1373,14 +1373,14 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="13">
+      <c r="B40" s="20">
         <v>209</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
       <c r="E40" s="3" t="s">
         <v>27</v>
       </c>
@@ -1389,10 +1389,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
       <c r="E41" s="3" t="s">
         <v>28</v>
       </c>
@@ -1401,10 +1401,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
       <c r="E42" s="3" t="s">
         <v>29</v>
       </c>
@@ -1413,16 +1413,16 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="13">
+      <c r="B43" s="20">
         <v>262</v>
       </c>
-      <c r="C43" s="14">
+      <c r="C43" s="21">
         <v>4600</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="17" t="s">
         <v>70</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1433,10 +1433,10 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="12"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="17"/>
       <c r="E44" s="3" t="s">
         <v>28</v>
       </c>
@@ -1445,10 +1445,10 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="12"/>
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="17"/>
       <c r="E45" s="3" t="s">
         <v>29</v>
       </c>
@@ -1457,14 +1457,14 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B46" s="20">
         <v>263</v>
       </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="12"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="17"/>
       <c r="E46" s="3" t="s">
         <v>27</v>
       </c>
@@ -1473,10 +1473,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="12"/>
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="17"/>
       <c r="E47" s="3" t="s">
         <v>28</v>
       </c>
@@ -1485,10 +1485,10 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="12"/>
+      <c r="A48" s="20"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="17"/>
       <c r="E48" s="3" t="s">
         <v>29</v>
       </c>
@@ -1497,14 +1497,14 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="13">
+      <c r="B49" s="20">
         <v>264</v>
       </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="12"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="17"/>
       <c r="E49" s="3" t="s">
         <v>27</v>
       </c>
@@ -1514,10 +1514,10 @@
       <c r="I49" s="8"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="12"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="17"/>
       <c r="E50" s="3" t="s">
         <v>28</v>
       </c>
@@ -1526,10 +1526,10 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="12"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="17"/>
       <c r="E51" s="3" t="s">
         <v>29</v>
       </c>
@@ -1538,16 +1538,16 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="13">
+      <c r="B52" s="20">
         <v>202</v>
       </c>
-      <c r="C52" s="12">
+      <c r="C52" s="17">
         <v>4600</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D52" s="17" t="s">
         <v>73</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -1558,10 +1558,10 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
       <c r="E53" s="3" t="s">
         <v>28</v>
       </c>
@@ -1570,10 +1570,10 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
+      <c r="A54" s="20"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
       <c r="E54" s="3" t="s">
         <v>29</v>
       </c>
@@ -1582,16 +1582,16 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="13">
+      <c r="B55" s="20">
         <v>394</v>
       </c>
-      <c r="C55" s="12">
+      <c r="C55" s="17">
         <v>4600</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="17" t="s">
         <v>77</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -1602,10 +1602,10 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
+      <c r="A56" s="20"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
       <c r="E56" s="3" t="s">
         <v>28</v>
       </c>
@@ -1614,10 +1614,10 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
       <c r="E57" s="3" t="s">
         <v>29</v>
       </c>
@@ -1626,16 +1626,16 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="13">
+      <c r="B58" s="20">
         <v>361</v>
       </c>
-      <c r="C58" s="12">
+      <c r="C58" s="17">
         <v>4600</v>
       </c>
-      <c r="D58" s="12"/>
+      <c r="D58" s="17"/>
       <c r="E58" s="3" t="s">
         <v>27</v>
       </c>
@@ -1644,10 +1644,10 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
+      <c r="A59" s="20"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
       <c r="E59" s="3" t="s">
         <v>28</v>
       </c>
@@ -1656,10 +1656,10 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="13"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
+      <c r="A60" s="20"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
       <c r="E60" s="3" t="s">
         <v>29</v>
       </c>
@@ -1668,16 +1668,16 @@
       </c>
     </row>
     <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B61" s="13">
+      <c r="B61" s="20">
         <v>364</v>
       </c>
-      <c r="C61" s="12">
+      <c r="C61" s="17">
         <v>4600</v>
       </c>
-      <c r="D61" s="12"/>
+      <c r="D61" s="17"/>
       <c r="E61" s="3" t="s">
         <v>27</v>
       </c>
@@ -1686,10 +1686,10 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
+      <c r="A62" s="20"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
       <c r="E62" s="3" t="s">
         <v>28</v>
       </c>
@@ -1698,10 +1698,10 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="13"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
+      <c r="A63" s="20"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
       <c r="E63" s="3" t="s">
         <v>29</v>
       </c>
@@ -1710,16 +1710,16 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B64" s="13">
+      <c r="B64" s="20">
         <v>366</v>
       </c>
-      <c r="C64" s="12">
+      <c r="C64" s="17">
         <v>4600</v>
       </c>
-      <c r="D64" s="12"/>
+      <c r="D64" s="17"/>
       <c r="E64" s="3" t="s">
         <v>27</v>
       </c>
@@ -1728,10 +1728,10 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
+      <c r="A65" s="20"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
       <c r="E65" s="3" t="s">
         <v>28</v>
       </c>
@@ -1740,10 +1740,10 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="13"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
+      <c r="A66" s="20"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
       <c r="E66" s="3" t="s">
         <v>29</v>
       </c>
@@ -1752,16 +1752,16 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="13" t="s">
+      <c r="A67" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B67" s="13">
+      <c r="B67" s="20">
         <v>393</v>
       </c>
-      <c r="C67" s="12">
+      <c r="C67" s="17">
         <v>4600</v>
       </c>
-      <c r="D67" s="12" t="s">
+      <c r="D67" s="17" t="s">
         <v>76</v>
       </c>
       <c r="E67" s="3" t="s">
@@ -1772,10 +1772,10 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="13"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
+      <c r="A68" s="20"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
       <c r="E68" s="3" t="s">
         <v>28</v>
       </c>
@@ -1784,10 +1784,10 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="13"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
+      <c r="A69" s="20"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
       <c r="E69" s="3" t="s">
         <v>29</v>
       </c>
@@ -1796,16 +1796,16 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B70" s="13">
+      <c r="B70" s="20">
         <v>215</v>
       </c>
-      <c r="C70" s="12">
+      <c r="C70" s="17">
         <v>4600</v>
       </c>
-      <c r="D70" s="12" t="s">
+      <c r="D70" s="17" t="s">
         <v>46</v>
       </c>
       <c r="E70" s="3" t="s">
@@ -1816,10 +1816,10 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="13"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
+      <c r="A71" s="20"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
       <c r="E71" s="3" t="s">
         <v>28</v>
       </c>
@@ -1828,10 +1828,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="13"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
+      <c r="A72" s="20"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
       <c r="E72" s="3" t="s">
         <v>29</v>
       </c>
@@ -1840,14 +1840,14 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="13" t="s">
+      <c r="A73" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B73" s="13">
+      <c r="B73" s="20">
         <v>243</v>
       </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
       <c r="E73" s="3" t="s">
         <v>27</v>
       </c>
@@ -1856,10 +1856,10 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="13"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
+      <c r="A74" s="20"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
       <c r="E74" s="3" t="s">
         <v>28</v>
       </c>
@@ -1868,10 +1868,10 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="13"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
+      <c r="A75" s="20"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
       <c r="E75" s="3" t="s">
         <v>29</v>
       </c>
@@ -1905,6 +1905,64 @@
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="D7:D21"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="D70:D75"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C21"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="D22:D30"/>
+    <mergeCell ref="D31:D42"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="D43:D51"/>
+    <mergeCell ref="C31:C42"/>
+    <mergeCell ref="C22:C30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="C43:C51"/>
+    <mergeCell ref="C70:C75"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:F1"/>
@@ -1921,64 +1979,6 @@
     <mergeCell ref="B67:B69"/>
     <mergeCell ref="C67:C69"/>
     <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="C43:C51"/>
-    <mergeCell ref="C70:C75"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="D22:D30"/>
-    <mergeCell ref="D31:D42"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="D43:D51"/>
-    <mergeCell ref="C31:C42"/>
-    <mergeCell ref="C22:C30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C21"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="D7:D21"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="D70:D75"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>